<commit_message>
Commented Stategy and Cleared Spreadsheets
</commit_message>
<xml_diff>
--- a/Timesheet_Report.xlsx
+++ b/Timesheet_Report.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apreza\Documents\GitHub\TimeReport\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="7" r:id="rId1"/>
+    <sheet name="10.24.2016" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Template" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+  <si>
+    <t>10.24.2016</t>
+  </si>
   <si>
     <t>Total</t>
   </si>
@@ -43,6 +42,78 @@
   </si>
   <si>
     <t>Saturday</t>
+  </si>
+  <si>
+    <t>Aljon Preza</t>
+  </si>
+  <si>
+    <t>Anna Fong</t>
+  </si>
+  <si>
+    <t>Austin Haruki</t>
+  </si>
+  <si>
+    <t>Brett Kimura</t>
+  </si>
+  <si>
+    <t>Caden Morikuni</t>
+  </si>
+  <si>
+    <t>Colin Goshi</t>
+  </si>
+  <si>
+    <t>Floyd Tanaka</t>
+  </si>
+  <si>
+    <t>Gary Murakami</t>
+  </si>
+  <si>
+    <t>James McDowell</t>
+  </si>
+  <si>
+    <t>Jeffrey Neimy</t>
+  </si>
+  <si>
+    <t>John Wingard</t>
+  </si>
+  <si>
+    <t>Justin Khan</t>
+  </si>
+  <si>
+    <t>Rashell Ito</t>
+  </si>
+  <si>
+    <t>Shirley Paoli</t>
+  </si>
+  <si>
+    <t>Terry Palomares</t>
+  </si>
+  <si>
+    <t>Torsten Vaivai-Soderberg</t>
+  </si>
+  <si>
+    <t>Consultants</t>
+  </si>
+  <si>
+    <t>Alfonso Torres</t>
+  </si>
+  <si>
+    <t>Amos Li</t>
+  </si>
+  <si>
+    <t>Luke Pu</t>
+  </si>
+  <si>
+    <t>Rex Li</t>
+  </si>
+  <si>
+    <t>Richard Yan</t>
+  </si>
+  <si>
+    <t>Rick Kooker</t>
+  </si>
+  <si>
+    <t>Totals</t>
   </si>
   <si>
     <t>Date</t>
@@ -51,40 +122,51 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="6">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="0"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="18"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -93,6 +175,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001F4E78"/>
+        <bgColor rgb="001F4E78"/>
       </patternFill>
     </fill>
   </fills>
@@ -106,31 +194,25 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="9">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="5" name="Percent" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -396,62 +478,344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.25" defaultRowHeight="15.75" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="5" width="24.75"/>
+    <col customWidth="1" max="2" min="2" style="5" width="8.25"/>
+    <col customWidth="1" max="3" min="3" style="5" width="8.75"/>
+    <col customWidth="1" max="4" min="4" style="5" width="10.25"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="23.45" r="1" s="5" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="n"/>
+      <c r="C1" s="3" t="n"/>
+      <c r="D1" s="3" t="n"/>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4">
+        <f>SUM(B4:G28)/COUNT(B4:G28)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="F2" s="2" t="n"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="8">
+        <f>SUM(B4:B28)/COUNT(B4:B28)</f>
+        <v/>
+      </c>
+      <c r="C29" s="8">
+        <f>SUM(C4:C28)/COUNT(C4:C28)</f>
+        <v/>
+      </c>
+      <c r="D29" s="8">
+        <f>SUM(D4:D28)/COUNT(D4:D28)</f>
+        <v/>
+      </c>
+      <c r="E29" s="8">
+        <f>SUM(E4:E28)/COUNT(E4:E28)</f>
+        <v/>
+      </c>
+      <c r="F29" s="8">
+        <f>SUM(F4:F28)/COUNT(F4:F28)</f>
+        <v/>
+      </c>
+      <c r="G29" s="8">
+        <f>SUM(G4:G28)/COUNT(G4:G28)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="98">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.25" defaultRowHeight="15.75" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="24.75" style="5" customWidth="1"/>
-    <col min="2" max="2" width="8.25" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.75" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="5" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="5" width="24.75"/>
+    <col customWidth="1" max="2" min="2" style="5" width="8.25"/>
+    <col customWidth="1" max="3" min="3" style="5" width="8.75"/>
+    <col customWidth="1" max="4" min="4" style="5" width="10.25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row customHeight="1" ht="23.45" r="1" s="5" spans="1:7">
       <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="n"/>
+      <c r="C1" s="3" t="n"/>
+      <c r="D1" s="3" t="n"/>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4">
+        <f>SUM(#REF!)/COUNT(#REF!)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="F2" s="2" t="n"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="4" t="e">
-        <f>SUM(#REF!)/COUNT(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Convert Intern Args String Instead of For Loop
workDayName is also now lower case to check intern schedule.
</commit_message>
<xml_diff>
--- a/Timesheet_Report.xlsx
+++ b/Timesheet_Report.xlsx
@@ -6,13 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="10.24.2016" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="10.17.2016" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="10.10.2016" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="10.03.2016" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="09.26.2016" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="09.19.2016" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Template" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="10.31.2016" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="10.24.2016" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="10.17.2016" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="10.10.2016" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="10.03.2016" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="09.26.2016" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="09.19.2016" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Template" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,99 +21,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+  <si>
+    <t>10.31.2016</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Employees</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Aljon Preza</t>
+  </si>
+  <si>
+    <t>Anna Fong</t>
+  </si>
+  <si>
+    <t>Austin Haruki</t>
+  </si>
+  <si>
+    <t>Brett Kimura</t>
+  </si>
+  <si>
+    <t>Caden Morikuni</t>
+  </si>
+  <si>
+    <t>Colin Goshi</t>
+  </si>
+  <si>
+    <t>Floyd Tanaka</t>
+  </si>
+  <si>
+    <t>Gary Murakami</t>
+  </si>
+  <si>
+    <t>James McDowell</t>
+  </si>
+  <si>
+    <t>Jeffrey Neimy</t>
+  </si>
+  <si>
+    <t>John Wingard</t>
+  </si>
+  <si>
+    <t>Justin Khan</t>
+  </si>
+  <si>
+    <t>Rashell Ito</t>
+  </si>
+  <si>
+    <t>Shirley Paoli</t>
+  </si>
+  <si>
+    <t>Terry Palomares</t>
+  </si>
+  <si>
+    <t>Torsten Vaivai-Soderberg</t>
+  </si>
+  <si>
+    <t>Consultants</t>
+  </si>
+  <si>
+    <t>Alfonso Torres</t>
+  </si>
+  <si>
+    <t>Amos Li</t>
+  </si>
+  <si>
+    <t>Jamie Nau</t>
+  </si>
+  <si>
+    <t>Luke Pu</t>
+  </si>
+  <si>
+    <t>Rex Li</t>
+  </si>
+  <si>
+    <t>Richard Yan</t>
+  </si>
+  <si>
+    <t>Rick Kooker</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
   <si>
     <t>10.24.2016</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Employees</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Anna Fong</t>
-  </si>
-  <si>
-    <t>Austin Haruki</t>
-  </si>
-  <si>
-    <t>Brett Kimura</t>
-  </si>
-  <si>
-    <t>Caden Morikuni</t>
-  </si>
-  <si>
-    <t>Colin Goshi</t>
-  </si>
-  <si>
-    <t>Floyd Tanaka</t>
-  </si>
-  <si>
-    <t>Gary Murakami</t>
-  </si>
-  <si>
-    <t>James McDowell</t>
-  </si>
-  <si>
-    <t>Jeffrey Neimy</t>
-  </si>
-  <si>
-    <t>John Wingard</t>
-  </si>
-  <si>
-    <t>Justin Khan</t>
-  </si>
-  <si>
-    <t>Rashell Ito</t>
-  </si>
-  <si>
-    <t>Shirley Paoli</t>
-  </si>
-  <si>
-    <t>Torsten Vaivai-Soderberg</t>
-  </si>
-  <si>
-    <t>Consultants</t>
-  </si>
-  <si>
-    <t>Alfonso Torres</t>
-  </si>
-  <si>
-    <t>Amos Li</t>
-  </si>
-  <si>
-    <t>Luke Pu</t>
-  </si>
-  <si>
-    <t>Rex Li</t>
-  </si>
-  <si>
-    <t>Richard Yan</t>
-  </si>
-  <si>
-    <t>Rick Kooker</t>
-  </si>
-  <si>
-    <t>Totals</t>
   </si>
   <si>
     <t>10.17.2016</t>
@@ -497,7 +510,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,7 +535,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="4">
-        <f>SUM(B4:G26)/COUNT(B4:G26)</f>
+        <f>SUM(B4:G29)/COUNT(B4:G29)</f>
         <v/>
       </c>
     </row>
@@ -557,19 +570,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -579,37 +580,13 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -619,18 +596,6 @@
       <c r="B7" t="n">
         <v>0</v>
       </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
@@ -639,36 +604,12 @@
       <c r="B8" t="n">
         <v>1</v>
       </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -677,19 +618,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -699,36 +628,12 @@
       <c r="B11" t="n">
         <v>1</v>
       </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -739,18 +644,6 @@
       <c r="B13" t="n">
         <v>1</v>
       </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
@@ -759,43 +652,19 @@
       <c r="B14" t="n">
         <v>1</v>
       </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>20</v>
       </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
@@ -804,44 +673,25 @@
       <c r="B17" t="n">
         <v>1</v>
       </c>
-      <c r="C17" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="C20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" t="n">
+      <c r="B19" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" t="s">
+      <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -849,38 +699,11 @@
       <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="C23" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
@@ -892,33 +715,47 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:7"/>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="8">
-        <f>SUM(B4:B26)/COUNT(B4:B26)</f>
-        <v/>
-      </c>
-      <c r="C27" s="8">
-        <f>SUM(C4:C26)/COUNT(C4:C26)</f>
-        <v/>
-      </c>
-      <c r="D27" s="8">
-        <f>SUM(D4:D26)/COUNT(D4:D26)</f>
-        <v/>
-      </c>
-      <c r="E27" s="8">
-        <f>SUM(E4:E26)/COUNT(E4:E26)</f>
-        <v/>
-      </c>
-      <c r="F27" s="8">
-        <f>SUM(F4:F26)/COUNT(F4:F26)</f>
-        <v/>
-      </c>
-      <c r="G27" s="8">
-        <f>SUM(G4:G26)/COUNT(G4:G26)</f>
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="8">
+        <f>SUM(B4:B29)/COUNT(B4:B29)</f>
+        <v/>
+      </c>
+      <c r="C30" s="8">
+        <f>SUM(C4:C29)/COUNT(C4:C29)</f>
+        <v/>
+      </c>
+      <c r="D30" s="8">
+        <f>SUM(D4:D29)/COUNT(D4:D29)</f>
+        <v/>
+      </c>
+      <c r="E30" s="8">
+        <f>SUM(E4:E29)/COUNT(E4:E29)</f>
+        <v/>
+      </c>
+      <c r="F30" s="8">
+        <f>SUM(F4:F29)/COUNT(F4:F29)</f>
+        <v/>
+      </c>
+      <c r="G30" s="8">
+        <f>SUM(G4:G29)/COUNT(G4:G29)</f>
         <v/>
       </c>
     </row>
@@ -949,7 +786,7 @@
   <sheetData>
     <row customHeight="1" ht="23.4" r="1" s="5" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B1" s="3" t="n"/>
       <c r="C1" s="3" t="n"/>
@@ -990,13 +827,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -1010,7 +847,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -1025,24 +862,24 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -1050,10 +887,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -1070,36 +907,36 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -1110,19 +947,19 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -1130,7 +967,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
@@ -1150,13 +987,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -1170,10 +1007,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
@@ -1190,16 +1027,16 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -1210,15 +1047,12 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -1238,7 +1072,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
@@ -1247,7 +1081,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -1258,12 +1092,12 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" t="n">
         <v>1</v>
@@ -1276,19 +1110,16 @@
       </c>
       <c r="F20" t="n">
         <v>1</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
@@ -1300,15 +1131,12 @@
         <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C23" t="n">
         <v>1</v>
@@ -1328,17 +1156,17 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B27" s="8">
         <f>SUM(B4:B26)/COUNT(B4:B26)</f>
@@ -1392,7 +1220,7 @@
   <sheetData>
     <row customHeight="1" ht="23.4" r="1" s="5" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" s="3" t="n"/>
       <c r="C1" s="3" t="n"/>
@@ -1433,13 +1261,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -1453,7 +1281,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -1473,19 +1301,19 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -1493,7 +1321,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -1513,10 +1341,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -1525,21 +1353,21 @@
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -1553,19 +1381,19 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -1573,7 +1401,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
@@ -1593,10 +1421,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -1613,13 +1441,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
@@ -1633,7 +1461,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -1645,7 +1473,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -1653,27 +1481,15 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -1693,16 +1509,16 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -1713,12 +1529,12 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" t="n">
         <v>1</v>
@@ -1733,32 +1549,17 @@
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
@@ -1778,67 +1579,37 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B27" s="8">
         <f>SUM(B4:B26)/COUNT(B4:B26)</f>
@@ -1876,7 +1647,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1892,7 +1663,7 @@
   <sheetData>
     <row customHeight="1" ht="23.4" r="1" s="5" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B1" s="3" t="n"/>
       <c r="C1" s="3" t="n"/>
@@ -1901,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="4">
-        <f>SUM(B4:G25)/COUNT(B4:G25)</f>
+        <f>SUM(B4:G26)/COUNT(B4:G26)</f>
         <v/>
       </c>
     </row>
@@ -1933,41 +1704,101 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1978,6 +1809,18 @@
       <c r="B9" t="n">
         <v>1</v>
       </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
@@ -1986,6 +1829,18 @@
       <c r="B10" t="n">
         <v>1</v>
       </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
@@ -1994,6 +1849,18 @@
       <c r="B11" t="n">
         <v>1</v>
       </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
@@ -2002,12 +1869,36 @@
       <c r="B12" t="n">
         <v>1</v>
       </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2018,13 +1909,37 @@
       <c r="B14" t="n">
         <v>0</v>
       </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2034,68 +1949,190 @@
       <c r="B16" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="6" t="s">
-        <v>23</v>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>24</v>
+      <c r="A19" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="8">
-        <f>SUM(B4:B25)/COUNT(B4:B25)</f>
-        <v/>
-      </c>
-      <c r="C26" s="8">
-        <f>SUM(C4:C25)/COUNT(C4:C25)</f>
-        <v/>
-      </c>
-      <c r="D26" s="8">
-        <f>SUM(D4:D25)/COUNT(D4:D25)</f>
-        <v/>
-      </c>
-      <c r="E26" s="8">
-        <f>SUM(E4:E25)/COUNT(E4:E25)</f>
-        <v/>
-      </c>
-      <c r="F26" s="8">
-        <f>SUM(F4:F25)/COUNT(F4:F25)</f>
-        <v/>
-      </c>
-      <c r="G26" s="8">
-        <f>SUM(G4:G25)/COUNT(G4:G25)</f>
+        <v>31</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="8">
+        <f>SUM(B4:B26)/COUNT(B4:B26)</f>
+        <v/>
+      </c>
+      <c r="C27" s="8">
+        <f>SUM(C4:C26)/COUNT(C4:C26)</f>
+        <v/>
+      </c>
+      <c r="D27" s="8">
+        <f>SUM(D4:D26)/COUNT(D4:D26)</f>
+        <v/>
+      </c>
+      <c r="E27" s="8">
+        <f>SUM(E4:E26)/COUNT(E4:E26)</f>
+        <v/>
+      </c>
+      <c r="F27" s="8">
+        <f>SUM(F4:F26)/COUNT(F4:F26)</f>
+        <v/>
+      </c>
+      <c r="G27" s="8">
+        <f>SUM(G4:G26)/COUNT(G4:G26)</f>
         <v/>
       </c>
     </row>
@@ -2126,7 +2163,7 @@
   <sheetData>
     <row customHeight="1" ht="23.4" r="1" s="5" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B1" s="3" t="n"/>
       <c r="C1" s="3" t="n"/>
@@ -2167,392 +2204,146 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B26" s="8">
         <f>SUM(B4:B25)/COUNT(B4:B25)</f>
@@ -2606,7 +2397,7 @@
   <sheetData>
     <row customHeight="1" ht="23.4" r="1" s="5" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3" t="n"/>
       <c r="C1" s="3" t="n"/>
@@ -2647,7 +2438,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -2667,7 +2458,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -2687,7 +2478,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -2707,7 +2498,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -2727,7 +2518,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -2747,7 +2538,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -2767,16 +2558,16 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -2787,7 +2578,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
@@ -2796,18 +2587,18 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -2816,7 +2607,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -2827,19 +2618,19 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -2847,7 +2638,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -2867,7 +2658,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" t="n">
         <v>1</v>
@@ -2887,7 +2678,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -2907,12 +2698,12 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
@@ -2932,7 +2723,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -2952,7 +2743,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C21" t="n">
         <v>1</v>
@@ -2972,7 +2763,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
@@ -2992,10 +2783,10 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
@@ -3004,15 +2795,15 @@
         <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -3032,7 +2823,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B26" s="8">
         <f>SUM(B4:B25)/COUNT(B4:B25)</f>
@@ -3065,6 +2856,486 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.19921875" defaultRowHeight="15.6" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="5" width="24.69921875"/>
+    <col customWidth="1" max="2" min="2" style="5" width="8.19921875"/>
+    <col customWidth="1" max="3" min="3" style="5" width="8.69921875"/>
+    <col customWidth="1" max="4" min="4" style="5" width="10.19921875"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="23.4" r="1" s="5" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="n"/>
+      <c r="C1" s="3" t="n"/>
+      <c r="D1" s="3" t="n"/>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4">
+        <f>SUM(B4:G25)/COUNT(B4:G25)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="F2" s="2" t="n"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="8">
+        <f>SUM(B4:B25)/COUNT(B4:B25)</f>
+        <v/>
+      </c>
+      <c r="C26" s="8">
+        <f>SUM(C4:C25)/COUNT(C4:C25)</f>
+        <v/>
+      </c>
+      <c r="D26" s="8">
+        <f>SUM(D4:D25)/COUNT(D4:D25)</f>
+        <v/>
+      </c>
+      <c r="E26" s="8">
+        <f>SUM(E4:E25)/COUNT(E4:E25)</f>
+        <v/>
+      </c>
+      <c r="F26" s="8">
+        <f>SUM(F4:F25)/COUNT(F4:F25)</f>
+        <v/>
+      </c>
+      <c r="G26" s="8">
+        <f>SUM(G4:G25)/COUNT(G4:G25)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3086,7 +3357,7 @@
   <sheetData>
     <row customHeight="1" ht="23.4" r="1" s="5" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B1" s="3" t="n"/>
       <c r="C1" s="3" t="n"/>

</xml_diff>